<commit_message>
atualização de diagramas de classe e adição de diagramas de sequencia para Login
</commit_message>
<xml_diff>
--- a/criaçãoTCC.xlsx
+++ b/criaçãoTCC.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -72,9 +72,24 @@
     <t>inserir, atualizar, excluir e consultar cadastro de usuários</t>
   </si>
   <si>
+    <t>O administrador ou usuário acessa o sistema, após o login, o usuário acessa a opção de vendas no menu , onde o sistema oferece a opção de gerar relatório  mensal e semanal.</t>
+  </si>
+  <si>
+    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção produtos no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do produto e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
     <t xml:space="preserve">O usuário ou administrador deve preencher com seu login e sua senha, para demostrar a entrada no sitema com suas respectivas restrições </t>
   </si>
   <si>
+    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do prduto e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
+    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados da categoria e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
+    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do fornecedor e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
     <t>Sprint Backlog</t>
   </si>
   <si>
@@ -108,6 +123,9 @@
     <t>etc...</t>
   </si>
   <si>
+    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do usuário e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
     <t>Fazer o digrama de sequência de todas as funções do crud</t>
   </si>
   <si>
@@ -117,61 +135,91 @@
     <t>Fazer o diagrama de sequência, sendo o pagamento com dinheiro o fluxo principal e pagamento com cartão o fluxo alternativo</t>
   </si>
   <si>
+    <t>Fazer diagrama de sequência, tendo gerar relatório mensal como fluxo principal e gerar relatório semanal com fluxo alternativo</t>
+  </si>
+  <si>
     <t>efetuar digrama de sequência como usuário simples e administrador, tendo um fluxo alternativo com usuário inválido e um com senha inválida</t>
   </si>
   <si>
+    <t>inserir, atualizar, excluir e consultar  de clientes</t>
+  </si>
+  <si>
     <t>Registrar Venda</t>
   </si>
   <si>
-    <t>Montar Diagrama de sequência</t>
-  </si>
-  <si>
-    <t>Criar método para CRUD</t>
-  </si>
-  <si>
-    <t>Definir Interface</t>
-  </si>
-  <si>
-    <t>Verificar estrutura BD</t>
-  </si>
-  <si>
-    <t>Testar e validar</t>
-  </si>
-  <si>
-    <t>Criar método para gerar cobrança</t>
-  </si>
-  <si>
-    <t>inserir, atualizar, excluir e consultar clientes</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema como administrador, o sistema exibirará então um menú de opções, selecionar a opção clientes no menu, após isso, na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do cliente  apoós a busca por nome ou CPFe na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu, após isso, na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do usuário após busca por CPF ou Login e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
-  </si>
-  <si>
-    <t>O usário administrador ou usuário simples acessa o sistema, após o login, o usuário acessa a opção de vendas no menu , onde o sistema oferece a opção de gerar relatório  mensal e semanal.</t>
-  </si>
-  <si>
-    <t>Fazer o digrama de sequência sendo o relatório mensal o fluxo básico e o semanal o fluxo alternativo</t>
-  </si>
-  <si>
-    <t>O  usuário administrador ou usuário simples acessa o sistema, após o login, e  acessa a opção de vendas no menu , onde o sistema oferece a opção de gerar gráfico  mensal e semanal.</t>
-  </si>
-  <si>
-    <t>Fazer diagrama de sequência, tendo gerar gáafico mensal como fluxo principal e gerar gráfico semanal como fluxo alternativo</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema, exibirará então um menú de opções, selecionar a opção produtos no menu, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do produto buscado pelo seu nome ou código, na opção atualizar, exibirá os campos para alteração e na opção excluir o produto é rmovido do sistema. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção categoria  após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados da categoria  consultada pelo seu código, na opção atualizar, exibirá os campos para alteração e na opção excluir removerá a categoria do sistema. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção usuários no menu e clicar em cadastrar, após isso, Na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do prduto consultado pelo su código, na opção atualizar, exibirá os campos para alteração e opção excluir removerá o produto do sistema. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
-  </si>
-  <si>
-    <t>Logar-se no sistema como administrador,o sistema exibirará então um menú de opções, selecionar a opção fornecedores no menu e, após isso, na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do fornecedor consultado pelo nome ou código e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+    <t>O administrador ou usuário acessa o sistema, após o login, o usuário acessa a opção de vendas no menu , onde o sistema oferece a opção de gerar gráfico  mensal e semanal.</t>
+  </si>
+  <si>
+    <t>Logar-se no sistema como administrador, o sistema exibirará então um menú de opções, selecionar a opção clientes no menu e clicar em cadastrar, após isso, na opção inserir, o sistema apresentará os campos a serem preenchidos para um novo cadastro, na opção consultar, ele mostrará os dados do cliente e na opção atualizar, exibirá os campos para alteração. O sistema deve reconhecer qual opção foi selecionada e executar de acordo com essa opção.</t>
+  </si>
+  <si>
+    <t>João Paulo Cruz Oliveira</t>
+  </si>
+  <si>
+    <t>Kevin Rangel Moreira</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Criação dos medodos para manter Produtos CRUD</t>
+  </si>
+  <si>
+    <t>Criação da interface</t>
+  </si>
+  <si>
+    <t>Verificar Estrutura BD</t>
+  </si>
+  <si>
+    <t>Efetuar testes iniciais</t>
+  </si>
+  <si>
+    <t>Criar metodo para finalizar venda</t>
+  </si>
+  <si>
+    <t>Criação de interface</t>
+  </si>
+  <si>
+    <t>Verificar Estrutura de BD</t>
+  </si>
+  <si>
+    <t>Efetuar Testes iniciais (teste unitário)</t>
+  </si>
+  <si>
+    <t>criar metodo para gerar permissão de acordo com login</t>
+  </si>
+  <si>
+    <t>Criar interface</t>
+  </si>
+  <si>
+    <t>Verificar estrutura do banco de dados</t>
+  </si>
+  <si>
+    <t>criar metodo manter cliente CRUD</t>
+  </si>
+  <si>
+    <t>Verificar estrutura de BD</t>
+  </si>
+  <si>
+    <t>Efetuar testes iniciais (teste unitário)</t>
+  </si>
+  <si>
+    <t>não iniciado</t>
+  </si>
+  <si>
+    <t>completo</t>
+  </si>
+  <si>
+    <t>Criar diagrama de Sequência Login</t>
+  </si>
+  <si>
+    <t>Criar diagrama de Sequência Vendda</t>
+  </si>
+  <si>
+    <t>Criar diagrama de sequênci manter Cliente</t>
+  </si>
+  <si>
+    <t>Criar diagrama de Sequência manter Produto</t>
   </si>
 </sst>
 </file>
@@ -356,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -382,6 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +770,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="345" x14ac:dyDescent="0.25">
@@ -741,10 +790,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -752,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9">
         <v>90</v>
@@ -761,13 +810,13 @@
         <v>5</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -781,13 +830,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -801,13 +850,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -821,10 +870,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -841,13 +890,13 @@
         <v>5</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="405" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -861,13 +910,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -881,10 +930,10 @@
         <v>5</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="345" x14ac:dyDescent="0.25">
@@ -901,10 +950,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -919,24 +968,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -950,105 +1000,137 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
+      <c r="A2" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="9">
+        <v>100</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="9">
+        <v>40</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="9">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="9">
+        <v>50</v>
+      </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="9">
+        <v>50</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -1060,12 +1142,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -1074,7 +1164,7 @@
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1089,37 +1179,37 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1130,12 +1220,20 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="9">
+        <v>100</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -1147,12 +1245,20 @@
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="9">
+        <v>40</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1164,12 +1270,20 @@
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="9">
+        <v>50</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -1181,12 +1295,20 @@
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="9">
+        <v>50</v>
+      </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -1198,12 +1320,20 @@
         <v>5</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1212,7 +1342,7 @@
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1227,37 +1357,37 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,12 +1398,20 @@
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="9">
+        <v>100</v>
+      </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1285,12 +1423,20 @@
         <v>2</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="9">
+        <v>3</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="9">
+        <v>40</v>
+      </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -1302,12 +1448,20 @@
         <v>3</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="9">
+        <v>50</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -1319,12 +1473,20 @@
         <v>4</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="9">
+        <v>2</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="9">
+        <v>50</v>
+      </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1336,17 +1498,201 @@
         <v>5</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="14">
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0</v>
+      </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="16"/>
     </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="9">
+        <v>100</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="9">
+        <v>2</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="9">
+        <v>3</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="9">
+        <v>40</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9">
+        <v>3</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="9">
+        <v>100</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="9">
+        <v>4</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="9">
+        <v>50</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="14">
+        <v>0</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>